<commit_message>
update script for PLP-PDP and launch URL
</commit_message>
<xml_diff>
--- a/resources/Automation_Data.xlsx
+++ b/resources/Automation_Data.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jjill-my.sharepoint.com/personal/nikhitha_muthukur_jjill_com/Documents/Automation/Projects/JjillRepository/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikhitha.muthukur\git\JjillTestRepository\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="6_{C8D0D2DC-6C4A-45DC-928B-04FEFC342446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11BB7C60-B3F5-449A-A254-EFDE44D9919F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3387A5DF-2386-4FE5-8773-AB108F8DDC18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{6BFA5E0A-9DDB-4471-A408-EA685EED7E6E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{6BFA5E0A-9DDB-4471-A408-EA685EED7E6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Address_Fields" sheetId="1" r:id="rId1"/>
     <sheet name="Login_Data" sheetId="2" r:id="rId2"/>
     <sheet name="Cards" sheetId="3" r:id="rId3"/>
     <sheet name="Search_Data" sheetId="4" r:id="rId4"/>
+    <sheet name="URL" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="73">
   <si>
     <t>Scenario</t>
   </si>
@@ -239,6 +240,375 @@
   <si>
     <t>123791</t>
   </si>
+  <si>
+    <t>URLNAME</t>
+  </si>
+  <si>
+    <t>Launch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://staging-ecomm.jjill.com/product/pure-jill-ballet-sleeve-tunic?color=780
+https://staging-ecomm.jjill.com/product/everyday-cotton-tee?color=6HA
+https://staging-ecomm.jjill.com/product/luxe-supima%C2%AE-pleat-back-tee?color=6TJ
+https://staging-ecomm.jjill.com/product/fit-french-terry-hooded-tunic?color=6EJ
+https://staging-ecomm.jjill.com/product/pure-jill-embroidered-jersey-tunic?color=6EC
+https://staging-ecomm.jjill.com/product/pure-jill-affinity-blouse?color=3RS
+https://staging-ecomm.jjill.com/product/pure-jill-embroidered-a-line-top?color=5ZR
+https://staging-ecomm.jjill.com/product/smocked-square-neck-top?color=6HJ
+https://staging-ecomm.jjill.com/product/ponte-convertible-tie-top?color=EZL
+https://staging-ecomm.jjill.com/product/smocked-henley-top?color=AXX
+https://staging-ecomm.jjill.com/product/mixed-florals-border-printed-top?color=6IH
+https://staging-ecomm.jjill.com/product/geometrically-embroidered-v-neck-tunic?color=6CQ
+https://staging-ecomm.jjill.com/product/long-sleeve-pima-crew-neck-tee?color=6ZV
+https://staging-ecomm.jjill.com/product/fit-french-terry-seamed-sweatshirt?color=AZN
+https://staging-ecomm.jjill.com/product/fit-hooded-snap-front-tunic?color=6EI
+https://staging-ecomm.jjill.com/product/fit-ultimate-fleece-collared-sweatshirt?color=871
+https://staging-ecomm.jjill.com/product/essential-forward-seam-tee?color=6TD
+https://staging-ecomm.jjill.com/product/twisted-hem-heathered-top?color=6SS
+https://staging-ecomm.jjill.com/product/striped-a-line-halter-top?color=6CC
+https://staging-ecomm.jjill.com/product/wearever-shirred-a-line-tunic?color=6DB
+https://staging-ecomm.jjill.com/product/pima-slub-elbow-sleeve-tee?color=0SY
+https://staging-ecomm.jjill.com/product/wearever-convertible-shoulder-top?color=31J
+https://staging-ecomm.jjill.com/product/wearever-double-face-jersey-seamed-tee?color=20M
+https://staging-ecomm.jjill.com/product/pure-jill-hemp-cotton-henley-top?color=61F
+https://staging-ecomm.jjill.com/product/pure-jill-space-dyed-tunic?color=347
+https://staging-ecomm.jjill.com/product/pure-jill-double-knit-seamed-tunic?color=6AW
+https://staging-ecomm.jjill.com/product/pure-jill-printed-soft-v-neck-top?color=6CZ
+https://staging-ecomm.jjill.com/product/pure-jill-banded-embroidered-tee?color=6SN
+https://staging-ecomm.jjill.com/product/wearever-convertible-shoulder-smocked-neck-top?color=6GS
+https://staging-ecomm.jjill.com/product/fit-progress-pima-stretch-shirttail-te-132651s-1?color=67Q
+https://staging-ecomm.jjill.com/product/pure-jill-ballet-sleeve-tunic?color=780
+https://staging-ecomm.jjill.com/product/everyday-cotton-tee?color=6HA
+https://staging-ecomm.jjill.com/product/luxe-supima%C2%AE-pleat-back-tee?color=6TJ
+https://staging-ecomm.jjill.com/product/fit-french-terry-hooded-tunic?color=6EJ
+https://staging-ecomm.jjill.com/product/pure-jill-embroidered-jersey-tunic?color=6EC
+https://staging-ecomm.jjill.com/product/pure-jill-affinity-blouse?color=3RS
+https://staging-ecomm.jjill.com/product/pure-jill-embroidered-a-line-top?color=5ZR
+https://staging-ecomm.jjill.com/product/smocked-square-neck-top?color=6HJ
+https://staging-ecomm.jjill.com/product/ponte-convertible-tie-top?color=EZL
+https://staging-ecomm.jjill.com/product/smocked-henley-top?color=AXX
+https://staging-ecomm.jjill.com/product/mixed-florals-border-printed-top?color=6IH
+https://staging-ecomm.jjill.com/product/geometrically-embroidered-v-neck-tunic?color=6CQ
+https://staging-ecomm.jjill.com/product/long-sleeve-pima-crew-neck-tee?color=6ZV
+https://staging-ecomm.jjill.com/product/fit-french-terry-seamed-sweatshirt?color=AZN
+https://staging-ecomm.jjill.com/product/fit-hooded-snap-front-tunic?color=6EI
+https://staging-ecomm.jjill.com/product/fit-ultimate-fleece-collared-sweatshirt?color=871
+https://staging-ecomm.jjill.com/product/essential-forward-seam-tee?color=6TD
+https://staging-ecomm.jjill.com/product/twisted-hem-heathered-top?color=6SS
+https://staging-ecomm.jjill.com/product/striped-a-line-halter-top?color=6CC
+https://staging-ecomm.jjill.com/product/wearever-shirred-a-line-tunic?color=6DB
+https://staging-ecomm.jjill.com/product/pima-slub-elbow-sleeve-tee?color=0SY
+https://staging-ecomm.jjill.com/product/wearever-convertible-shoulder-top?color=31J
+https://staging-ecomm.jjill.com/product/wearever-double-face-jersey-seamed-tee?color=20M
+https://staging-ecomm.jjill.com/product/pure-jill-hemp-cotton-henley-top?color=61F
+https://staging-ecomm.jjill.com/product/pure-jill-space-dyed-tunic?color=347
+https://staging-ecomm.jjill.com/product/pure-jill-double-knit-seamed-tunic?color=6AW
+https://staging-ecomm.jjill.com/product/pure-jill-printed-soft-v-neck-top?color=6CZ
+https://staging-ecomm.jjill.com/product/pure-jill-banded-embroidered-tee?color=6SN
+https://staging-ecomm.jjill.com/product/wearever-convertible-shoulder-smocked-neck-top?color=6GS
+https://staging-ecomm.jjill.com/product/fit-progress-pima-stretch-shirttail-te-132651s-1?color=67Q
+https://staging-ecomm.jjill.com/product/pure-jill-ballet-sleeve-tunic?color=780
+https://staging-ecomm.jjill.com/product/everyday-cotton-tee?color=6HA
+https://staging-ecomm.jjill.com/product/luxe-supima%C2%AE-pleat-back-tee?color=6TJ
+https://staging-ecomm.jjill.com/product/fit-french-terry-hooded-tunic?color=6EJ
+https://staging-ecomm.jjill.com/product/pure-jill-embroidered-jersey-tunic?color=6EC
+https://staging-ecomm.jjill.com/product/pure-jill-affinity-blouse?color=3RS
+https://staging-ecomm.jjill.com/product/pure-jill-embroidered-a-line-top?color=5ZR
+https://staging-ecomm.jjill.com/product/smocked-square-neck-top?color=6HJ
+https://staging-ecomm.jjill.com/product/ponte-convertible-tie-top?color=EZL
+https://staging-ecomm.jjill.com/product/smocked-henley-top?color=AXX
+https://staging-ecomm.jjill.com/product/mixed-florals-border-printed-top?color=6IH
+https://staging-ecomm.jjill.com/product/geometrically-embroidered-v-neck-tunic?color=6CQ
+https://staging-ecomm.jjill.com/product/long-sleeve-pima-crew-neck-tee?color=6ZV
+https://staging-ecomm.jjill.com/product/fit-french-terry-seamed-sweatshirt?color=AZN
+https://staging-ecomm.jjill.com/product/fit-hooded-snap-front-tunic?color=6EI
+https://staging-ecomm.jjill.com/product/fit-ultimate-fleece-collared-sweatshirt?color=871
+https://staging-ecomm.jjill.com/product/essential-forward-seam-tee?color=6TD
+https://staging-ecomm.jjill.com/product/twisted-hem-heathered-top?color=6SS
+https://staging-ecomm.jjill.com/product/striped-a-line-halter-top?color=6CC
+https://staging-ecomm.jjill.com/product/wearever-shirred-a-line-tunic?color=6DB
+https://staging-ecomm.jjill.com/product/pima-slub-elbow-sleeve-tee?color=0SY
+https://staging-ecomm.jjill.com/product/wearever-convertible-shoulder-top?color=31J
+https://staging-ecomm.jjill.com/product/wearever-double-face-jersey-seamed-tee?color=20M
+https://staging-ecomm.jjill.com/product/pure-jill-hemp-cotton-henley-top?color=61F
+https://staging-ecomm.jjill.com/product/pure-jill-space-dyed-tunic?color=347
+https://staging-ecomm.jjill.com/product/pure-jill-double-knit-seamed-tunic?color=6AW
+https://staging-ecomm.jjill.com/product/pure-jill-printed-soft-v-neck-top?color=6CZ
+https://staging-ecomm.jjill.com/product/pure-jill-banded-embroidered-tee?color=6SN
+https://staging-ecomm.jjill.com/product/wearever-convertible-shoulder-smocked-neck-top?color=6GS
+https://staging-ecomm.jjill.com/product/fit-progress-pima-stretch-shirttail-te-132651s-1?color=67Q
+https://staging-ecomm.jjill.com/product/pure-jill-ballet-sleeve-tunic?color=780
+https://staging-ecomm.jjill.com/product/everyday-cotton-tee?color=6HA
+https://staging-ecomm.jjill.com/product/luxe-supima%C2%AE-pleat-back-tee?color=6TJ
+https://staging-ecomm.jjill.com/product/fit-french-terry-hooded-tunic?color=6EJ
+https://staging-ecomm.jjill.com/product/pure-jill-embroidered-jersey-tunic?color=6EC
+https://staging-ecomm.jjill.com/product/pure-jill-affinity-blouse?color=3RS
+https://staging-ecomm.jjill.com/product/pure-jill-embroidered-a-line-top?color=5ZR
+https://staging-ecomm.jjill.com/product/smocked-square-neck-top?color=6HJ
+https://staging-ecomm.jjill.com/product/ponte-convertible-tie-top?color=EZL
+https://staging-ecomm.jjill.com/product/smocked-henley-top?color=AXX
+https://staging-ecomm.jjill.com/product/mixed-florals-border-printed-top?color=6IH
+https://staging-ecomm.jjill.com/product/geometrically-embroidered-v-neck-tunic?color=6CQ
+https://staging-ecomm.jjill.com/product/long-sleeve-pima-crew-neck-tee?color=6ZV
+https://staging-ecomm.jjill.com/product/fit-french-terry-seamed-sweatshirt?color=AZN
+https://staging-ecomm.jjill.com/product/fit-hooded-snap-front-tunic?color=6EI
+https://staging-ecomm.jjill.com/product/fit-ultimate-fleece-collared-sweatshirt?color=871
+https://staging-ecomm.jjill.com/product/essential-forward-seam-tee?color=6TD
+https://staging-ecomm.jjill.com/product/twisted-hem-heathered-top?color=6SS
+https://staging-ecomm.jjill.com/product/striped-a-line-halter-top?color=6CC
+https://staging-ecomm.jjill.com/product/wearever-shirred-a-line-tunic?color=6DB
+https://staging-ecomm.jjill.com/product/pima-slub-elbow-sleeve-tee?color=0SY
+https://staging-ecomm.jjill.com/product/wearever-convertible-shoulder-top?color=31J
+https://staging-ecomm.jjill.com/product/wearever-double-face-jersey-seamed-tee?color=20M
+https://staging-ecomm.jjill.com/product/pure-jill-hemp-cotton-henley-top?color=61F
+https://staging-ecomm.jjill.com/product/pure-jill-space-dyed-tunic?color=347
+https://staging-ecomm.jjill.com/product/pure-jill-double-knit-seamed-tunic?color=6AW
+https://staging-ecomm.jjill.com/product/pure-jill-printed-soft-v-neck-top?color=6CZ
+https://staging-ecomm.jjill.com/product/pure-jill-banded-embroidered-tee?color=6SN
+https://staging-ecomm.jjill.com/product/wearever-convertible-shoulder-smocked-neck-top?color=6GS
+https://staging-ecomm.jjill.com/product/fit-progress-pima-stretch-shirttail-te-132651s-1?color=67Q
+https://staging-ecomm.jjill.com/product/pure-jill-ballet-sleeve-tunic?color=780
+https://staging-ecomm.jjill.com/product/everyday-cotton-tee?color=6HA
+https://staging-ecomm.jjill.com/product/luxe-supima%C2%AE-pleat-back-tee?color=6TJ
+https://staging-ecomm.jjill.com/product/fit-french-terry-hooded-tunic?color=6EJ
+https://staging-ecomm.jjill.com/product/pure-jill-embroidered-jersey-tunic?color=6EC
+https://staging-ecomm.jjill.com/product/pure-jill-affinity-blouse?color=3RS
+https://staging-ecomm.jjill.com/product/pure-jill-embroidered-a-line-top?color=5ZR
+https://staging-ecomm.jjill.com/product/smocked-square-neck-top?color=6HJ
+https://staging-ecomm.jjill.com/product/ponte-convertible-tie-top?color=EZL
+https://staging-ecomm.jjill.com/product/smocked-henley-top?color=AXX
+https://staging-ecomm.jjill.com/product/mixed-florals-border-printed-top?color=6IH
+https://staging-ecomm.jjill.com/product/geometrically-embroidered-v-neck-tunic?color=6CQ
+https://staging-ecomm.jjill.com/product/long-sleeve-pima-crew-neck-tee?color=6ZV
+https://staging-ecomm.jjill.com/product/fit-french-terry-seamed-sweatshirt?color=AZN
+https://staging-ecomm.jjill.com/product/fit-hooded-snap-front-tunic?color=6EI
+https://staging-ecomm.jjill.com/product/fit-ultimate-fleece-collared-sweatshirt?color=871
+https://staging-ecomm.jjill.com/product/essential-forward-seam-tee?color=6TD
+https://staging-ecomm.jjill.com/product/twisted-hem-heathered-top?color=6SS
+https://staging-ecomm.jjill.com/product/striped-a-line-halter-top?color=6CC
+https://staging-ecomm.jjill.com/product/wearever-shirred-a-line-tunic?color=6DB
+https://staging-ecomm.jjill.com/product/pima-slub-elbow-sleeve-tee?color=0SY
+https://staging-ecomm.jjill.com/product/wearever-convertible-shoulder-top?color=31J
+https://staging-ecomm.jjill.com/product/wearever-double-face-jersey-seamed-tee?color=20M
+https://staging-ecomm.jjill.com/product/pure-jill-hemp-cotton-henley-top?color=61F
+https://staging-ecomm.jjill.com/product/pure-jill-space-dyed-tunic?color=347
+https://staging-ecomm.jjill.com/product/pure-jill-double-knit-seamed-tunic?color=6AW
+https://staging-ecomm.jjill.com/product/pure-jill-printed-soft-v-neck-top?color=6CZ
+https://staging-ecomm.jjill.com/product/pure-jill-banded-embroidered-tee?color=6SN
+https://staging-ecomm.jjill.com/product/wearever-convertible-shoulder-smocked-neck-top?color=6GS
+https://staging-ecomm.jjill.com/product/fit-progress-pima-stretch-shirttail-te-132651s-1?color=67Q
+https://staging-ecomm.jjill.com/product/pure-jill-ballet-sleeve-tunic?color=780
+https://staging-ecomm.jjill.com/product/everyday-cotton-tee?color=6HA
+https://staging-ecomm.jjill.com/product/luxe-supima%C2%AE-pleat-back-tee?color=6TJ
+https://staging-ecomm.jjill.com/product/fit-french-terry-hooded-tunic?color=6EJ
+https://staging-ecomm.jjill.com/product/pure-jill-embroidered-jersey-tunic?color=6EC
+https://staging-ecomm.jjill.com/product/pure-jill-affinity-blouse?color=3RS
+https://staging-ecomm.jjill.com/product/pure-jill-embroidered-a-line-top?color=5ZR
+https://staging-ecomm.jjill.com/product/smocked-square-neck-top?color=6HJ
+https://staging-ecomm.jjill.com/product/ponte-convertible-tie-top?color=EZL
+https://staging-ecomm.jjill.com/product/smocked-henley-top?color=AXX
+https://staging-ecomm.jjill.com/product/mixed-florals-border-printed-top?color=6IH
+https://staging-ecomm.jjill.com/product/geometrically-embroidered-v-neck-tunic?color=6CQ
+https://staging-ecomm.jjill.com/product/long-sleeve-pima-crew-neck-tee?color=6ZV
+https://staging-ecomm.jjill.com/product/fit-french-terry-seamed-sweatshirt?color=AZN
+https://staging-ecomm.jjill.com/product/fit-hooded-snap-front-tunic?color=6EI
+https://staging-ecomm.jjill.com/product/fit-ultimate-fleece-collared-sweatshirt?color=871
+https://staging-ecomm.jjill.com/product/essential-forward-seam-tee?color=6TD
+https://staging-ecomm.jjill.com/product/twisted-hem-heathered-top?color=6SS
+https://staging-ecomm.jjill.com/product/striped-a-line-halter-top?color=6CC
+https://staging-ecomm.jjill.com/product/wearever-shirred-a-line-tunic?color=6DB
+https://staging-ecomm.jjill.com/product/pima-slub-elbow-sleeve-tee?color=0SY
+https://staging-ecomm.jjill.com/product/wearever-convertible-shoulder-top?color=31J
+https://staging-ecomm.jjill.com/product/wearever-double-face-jersey-seamed-tee?color=20M
+https://staging-ecomm.jjill.com/product/pure-jill-hemp-cotton-henley-top?color=61F
+https://staging-ecomm.jjill.com/product/pure-jill-space-dyed-tunic?color=347
+https://staging-ecomm.jjill.com/product/pure-jill-double-knit-seamed-tunic?color=6AW
+https://staging-ecomm.jjill.com/product/pure-jill-printed-soft-v-neck-top?color=6CZ
+https://staging-ecomm.jjill.com/product/pure-jill-banded-embroidered-tee?color=6SN
+https://staging-ecomm.jjill.com/product/wearever-convertible-shoulder-smocked-neck-top?color=6GS
+https://staging-ecomm.jjill.com/product/fit-progress-pima-stretch-shirttail-te-132651s-1?color=67Q
+https://staging-ecomm.jjill.com/product/pure-jill-ballet-sleeve-tunic?color=780
+https://staging-ecomm.jjill.com/product/everyday-cotton-tee?color=6HA
+https://staging-ecomm.jjill.com/product/luxe-supima%C2%AE-pleat-back-tee?color=6TJ
+https://staging-ecomm.jjill.com/product/fit-french-terry-hooded-tunic?color=6EJ
+https://staging-ecomm.jjill.com/product/pure-jill-embroidered-jersey-tunic?color=6EC
+https://staging-ecomm.jjill.com/product/pure-jill-affinity-blouse?color=3RS
+https://staging-ecomm.jjill.com/product/pure-jill-embroidered-a-line-top?color=5ZR
+https://staging-ecomm.jjill.com/product/smocked-square-neck-top?color=6HJ
+https://staging-ecomm.jjill.com/product/ponte-convertible-tie-top?color=EZL
+https://staging-ecomm.jjill.com/product/smocked-henley-top?color=AXX
+https://staging-ecomm.jjill.com/product/mixed-florals-border-printed-top?color=6IH
+https://staging-ecomm.jjill.com/product/geometrically-embroidered-v-neck-tunic?color=6CQ
+https://staging-ecomm.jjill.com/product/long-sleeve-pima-crew-neck-tee?color=6ZV
+https://staging-ecomm.jjill.com/product/fit-french-terry-seamed-sweatshirt?color=AZN
+https://staging-ecomm.jjill.com/product/fit-hooded-snap-front-tunic?color=6EI
+https://staging-ecomm.jjill.com/product/fit-ultimate-fleece-collared-sweatshirt?color=871
+https://staging-ecomm.jjill.com/product/essential-forward-seam-tee?color=6TD
+https://staging-ecomm.jjill.com/product/twisted-hem-heathered-top?color=6SS
+https://staging-ecomm.jjill.com/product/striped-a-line-halter-top?color=6CC
+https://staging-ecomm.jjill.com/product/wearever-shirred-a-line-tunic?color=6DB
+https://staging-ecomm.jjill.com/product/pima-slub-elbow-sleeve-tee?color=0SY
+https://staging-ecomm.jjill.com/product/wearever-convertible-shoulder-top?color=31J
+https://staging-ecomm.jjill.com/product/wearever-double-face-jersey-seamed-tee?color=20M
+https://staging-ecomm.jjill.com/product/pure-jill-hemp-cotton-henley-top?color=61F
+https://staging-ecomm.jjill.com/product/pure-jill-space-dyed-tunic?color=347
+https://staging-ecomm.jjill.com/product/pure-jill-double-knit-seamed-tunic?color=6AW
+https://staging-ecomm.jjill.com/product/pure-jill-printed-soft-v-neck-top?color=6CZ
+https://staging-ecomm.jjill.com/product/pure-jill-banded-embroidered-tee?color=6SN
+https://staging-ecomm.jjill.com/product/wearever-convertible-shoulder-smocked-neck-top?color=6GS
+https://staging-ecomm.jjill.com/product/fit-progress-pima-stretch-shirttail-te-132651s-1?color=67Q
+https://staging-ecomm.jjill.com/product/pure-jill-ballet-sleeve-tunic?color=780
+https://staging-ecomm.jjill.com/product/everyday-cotton-tee?color=6HA
+https://staging-ecomm.jjill.com/product/luxe-supima%C2%AE-pleat-back-tee?color=6TJ
+https://staging-ecomm.jjill.com/product/fit-french-terry-hooded-tunic?color=6EJ
+https://staging-ecomm.jjill.com/product/pure-jill-embroidered-jersey-tunic?color=6EC
+https://staging-ecomm.jjill.com/product/pure-jill-affinity-blouse?color=3RS
+https://staging-ecomm.jjill.com/product/pure-jill-embroidered-a-line-top?color=5ZR
+https://staging-ecomm.jjill.com/product/smocked-square-neck-top?color=6HJ
+https://staging-ecomm.jjill.com/product/ponte-convertible-tie-top?color=EZL
+https://staging-ecomm.jjill.com/product/smocked-henley-top?color=AXX
+https://staging-ecomm.jjill.com/product/mixed-florals-border-printed-top?color=6IH
+https://staging-ecomm.jjill.com/product/geometrically-embroidered-v-neck-tunic?color=6CQ
+https://staging-ecomm.jjill.com/product/long-sleeve-pima-crew-neck-tee?color=6ZV
+https://staging-ecomm.jjill.com/product/fit-french-terry-seamed-sweatshirt?color=AZN
+https://staging-ecomm.jjill.com/product/fit-hooded-snap-front-tunic?color=6EI
+https://staging-ecomm.jjill.com/product/fit-ultimate-fleece-collared-sweatshirt?color=871
+https://staging-ecomm.jjill.com/product/essential-forward-seam-tee?color=6TD
+https://staging-ecomm.jjill.com/product/twisted-hem-heathered-top?color=6SS
+https://staging-ecomm.jjill.com/product/striped-a-line-halter-top?color=6CC
+https://staging-ecomm.jjill.com/product/wearever-shirred-a-line-tunic?color=6DB
+https://staging-ecomm.jjill.com/product/pima-slub-elbow-sleeve-tee?color=0SY
+https://staging-ecomm.jjill.com/product/wearever-convertible-shoulder-top?color=31J
+https://staging-ecomm.jjill.com/product/wearever-double-face-jersey-seamed-tee?color=20M
+https://staging-ecomm.jjill.com/product/pure-jill-hemp-cotton-henley-top?color=61F
+https://staging-ecomm.jjill.com/product/pure-jill-space-dyed-tunic?color=347
+https://staging-ecomm.jjill.com/product/pure-jill-double-knit-seamed-tunic?color=6AW
+https://staging-ecomm.jjill.com/product/pure-jill-printed-soft-v-neck-top?color=6CZ
+https://staging-ecomm.jjill.com/product/pure-jill-banded-embroidered-tee?color=6SN
+https://staging-ecomm.jjill.com/product/wearever-convertible-shoulder-smocked-neck-top?color=6GS
+https://staging-ecomm.jjill.com/product/fit-progress-pima-stretch-shirttail-te-132651s-1?color=67Q
+https://staging-ecomm.jjill.com/product/pure-jill-ballet-sleeve-tunic?color=780
+https://staging-ecomm.jjill.com/product/everyday-cotton-tee?color=6HA
+https://staging-ecomm.jjill.com/product/luxe-supima%C2%AE-pleat-back-tee?color=6TJ
+https://staging-ecomm.jjill.com/product/fit-french-terry-hooded-tunic?color=6EJ
+https://staging-ecomm.jjill.com/product/pure-jill-embroidered-jersey-tunic?color=6EC
+https://staging-ecomm.jjill.com/product/pure-jill-affinity-blouse?color=3RS
+https://staging-ecomm.jjill.com/product/pure-jill-embroidered-a-line-top?color=5ZR
+https://staging-ecomm.jjill.com/product/smocked-square-neck-top?color=6HJ
+https://staging-ecomm.jjill.com/product/ponte-convertible-tie-top?color=EZL
+https://staging-ecomm.jjill.com/product/smocked-henley-top?color=AXX
+https://staging-ecomm.jjill.com/product/mixed-florals-border-printed-top?color=6IH
+https://staging-ecomm.jjill.com/product/geometrically-embroidered-v-neck-tunic?color=6CQ
+https://staging-ecomm.jjill.com/product/long-sleeve-pima-crew-neck-tee?color=6ZV
+https://staging-ecomm.jjill.com/product/fit-french-terry-seamed-sweatshirt?color=AZN
+https://staging-ecomm.jjill.com/product/fit-hooded-snap-front-tunic?color=6EI
+https://staging-ecomm.jjill.com/product/fit-ultimate-fleece-collared-sweatshirt?color=871
+https://staging-ecomm.jjill.com/product/essential-forward-seam-tee?color=6TD
+https://staging-ecomm.jjill.com/product/twisted-hem-heathered-top?color=6SS
+https://staging-ecomm.jjill.com/product/striped-a-line-halter-top?color=6CC
+https://staging-ecomm.jjill.com/product/wearever-shirred-a-line-tunic?color=6DB
+https://staging-ecomm.jjill.com/product/pima-slub-elbow-sleeve-tee?color=0SY
+https://staging-ecomm.jjill.com/product/wearever-convertible-shoulder-top?color=31J
+https://staging-ecomm.jjill.com/product/wearever-double-face-jersey-seamed-tee?color=20M
+https://staging-ecomm.jjill.com/product/pure-jill-hemp-cotton-henley-top?color=61F
+https://staging-ecomm.jjill.com/product/pure-jill-space-dyed-tunic?color=347
+https://staging-ecomm.jjill.com/product/pure-jill-double-knit-seamed-tunic?color=6AW
+https://staging-ecomm.jjill.com/product/pure-jill-printed-soft-v-neck-top?color=6CZ
+https://staging-ecomm.jjill.com/product/pure-jill-banded-embroidered-tee?color=6SN
+https://staging-ecomm.jjill.com/product/wearever-convertible-shoulder-smocked-neck-top?color=6GS
+https://staging-ecomm.jjill.com/product/fit-progress-pima-stretch-shirttail-te-132651s-1?color=67Q
+https://staging-ecomm.jjill.com/product/pure-jill-ballet-sleeve-tunic?color=780
+https://staging-ecomm.jjill.com/product/everyday-cotton-tee?color=6HA
+https://staging-ecomm.jjill.com/product/luxe-supima%C2%AE-pleat-back-tee?color=6TJ
+https://staging-ecomm.jjill.com/product/fit-french-terry-hooded-tunic?color=6EJ
+https://staging-ecomm.jjill.com/product/pure-jill-embroidered-jersey-tunic?color=6EC
+https://staging-ecomm.jjill.com/product/pure-jill-affinity-blouse?color=3RS
+https://staging-ecomm.jjill.com/product/pure-jill-embroidered-a-line-top?color=5ZR
+https://staging-ecomm.jjill.com/product/smocked-square-neck-top?color=6HJ
+https://staging-ecomm.jjill.com/product/ponte-convertible-tie-top?color=EZL
+https://staging-ecomm.jjill.com/product/smocked-henley-top?color=AXX
+https://staging-ecomm.jjill.com/product/mixed-florals-border-printed-top?color=6IH
+https://staging-ecomm.jjill.com/product/geometrically-embroidered-v-neck-tunic?color=6CQ
+https://staging-ecomm.jjill.com/product/long-sleeve-pima-crew-neck-tee?color=6ZV
+https://staging-ecomm.jjill.com/product/fit-french-terry-seamed-sweatshirt?color=AZN
+https://staging-ecomm.jjill.com/product/fit-hooded-snap-front-tunic?color=6EI
+https://staging-ecomm.jjill.com/product/fit-ultimate-fleece-collared-sweatshirt?color=871
+https://staging-ecomm.jjill.com/product/essential-forward-seam-tee?color=6TD
+https://staging-ecomm.jjill.com/product/twisted-hem-heathered-top?color=6SS
+https://staging-ecomm.jjill.com/product/striped-a-line-halter-top?color=6CC
+https://staging-ecomm.jjill.com/product/wearever-shirred-a-line-tunic?color=6DB
+https://staging-ecomm.jjill.com/product/pima-slub-elbow-sleeve-tee?color=0SY
+https://staging-ecomm.jjill.com/product/wearever-convertible-shoulder-top?color=31J
+https://staging-ecomm.jjill.com/product/wearever-double-face-jersey-seamed-tee?color=20M
+https://staging-ecomm.jjill.com/product/pure-jill-hemp-cotton-henley-top?color=61F
+https://staging-ecomm.jjill.com/product/pure-jill-space-dyed-tunic?color=347
+https://staging-ecomm.jjill.com/product/pure-jill-double-knit-seamed-tunic?color=6AW
+https://staging-ecomm.jjill.com/product/pure-jill-printed-soft-v-neck-top?color=6CZ
+https://staging-ecomm.jjill.com/product/pure-jill-banded-embroidered-tee?color=6SN
+https://staging-ecomm.jjill.com/product/wearever-convertible-shoulder-smocked-neck-top?color=6GS
+https://staging-ecomm.jjill.com/product/fit-progress-pima-stretch-shirttail-te-132651s-1?color=67Q
+https://staging-ecomm.jjill.com/product/pure-jill-ballet-sleeve-tunic?color=780
+https://staging-ecomm.jjill.com/product/everyday-cotton-tee?color=6HA
+https://staging-ecomm.jjill.com/product/luxe-supima%C2%AE-pleat-back-tee?color=6TJ
+https://staging-ecomm.jjill.com/product/fit-french-terry-hooded-tunic?color=6EJ
+https://staging-ecomm.jjill.com/product/pure-jill-embroidered-jersey-tunic?color=6EC
+https://staging-ecomm.jjill.com/product/pure-jill-affinity-blouse?color=3RS
+https://staging-ecomm.jjill.com/product/pure-jill-embroidered-a-line-top?color=5ZR
+https://staging-ecomm.jjill.com/product/smocked-square-neck-top?color=6HJ
+https://staging-ecomm.jjill.com/product/ponte-convertible-tie-top?color=EZL
+https://staging-ecomm.jjill.com/product/smocked-henley-top?color=AXX
+https://staging-ecomm.jjill.com/product/mixed-florals-border-printed-top?color=6IH
+https://staging-ecomm.jjill.com/product/geometrically-embroidered-v-neck-tunic?color=6CQ
+https://staging-ecomm.jjill.com/product/long-sleeve-pima-crew-neck-tee?color=6ZV
+https://staging-ecomm.jjill.com/product/fit-french-terry-seamed-sweatshirt?color=AZN
+https://staging-ecomm.jjill.com/product/fit-hooded-snap-front-tunic?color=6EI
+https://staging-ecomm.jjill.com/product/fit-ultimate-fleece-collared-sweatshirt?color=871
+https://staging-ecomm.jjill.com/product/essential-forward-seam-tee?color=6TD
+https://staging-ecomm.jjill.com/product/twisted-hem-heathered-top?color=6SS
+https://staging-ecomm.jjill.com/product/striped-a-line-halter-top?color=6CC
+https://staging-ecomm.jjill.com/product/wearever-shirred-a-line-tunic?color=6DB
+https://staging-ecomm.jjill.com/product/pima-slub-elbow-sleeve-tee?color=0SY
+https://staging-ecomm.jjill.com/product/wearever-convertible-shoulder-top?color=31J
+https://staging-ecomm.jjill.com/product/wearever-double-face-jersey-seamed-tee?color=20M
+https://staging-ecomm.jjill.com/product/pure-jill-hemp-cotton-henley-top?color=61F
+https://staging-ecomm.jjill.com/product/pure-jill-space-dyed-tunic?color=347
+https://staging-ecomm.jjill.com/product/pure-jill-double-knit-seamed-tunic?color=6AW
+https://staging-ecomm.jjill.com/product/pure-jill-printed-soft-v-neck-top?color=6CZ
+https://staging-ecomm.jjill.com/product/pure-jill-banded-embroidered-tee?color=6SN
+https://staging-ecomm.jjill.com/product/wearever-convertible-shoulder-smocked-neck-top?color=6GS
+https://staging-ecomm.jjill.com/product/fit-progress-pima-stretch-shirttail-te-132651s-1?color=67Q
+https://staging-ecomm.jjill.com/product/pure-jill-ballet-sleeve-tunic?color=780
+https://staging-ecomm.jjill.com/product/everyday-cotton-tee?color=6HA
+https://staging-ecomm.jjill.com/product/luxe-supima%C2%AE-pleat-back-tee?color=6TJ
+https://staging-ecomm.jjill.com/product/fit-french-terry-hooded-tunic?color=6EJ
+https://staging-ecomm.jjill.com/product/pure-jill-embroidered-jersey-tunic?color=6EC
+https://staging-ecomm.jjill.com/product/pure-jill-affinity-blouse?color=3RS
+https://staging-ecomm.jjill.com/product/pure-jill-embroidered-a-line-top?color=5ZR
+https://staging-ecomm.jjill.com/product/smocked-square-neck-top?color=6HJ
+https://staging-ecomm.jjill.com/product/ponte-convertible-tie-top?color=EZL
+https://staging-ecomm.jjill.com/product/smocked-henley-top?color=AXX
+https://staging-ecomm.jjill.com/product/mixed-florals-border-printed-top?color=6IH
+https://staging-ecomm.jjill.com/product/geometrically-embroidered-v-neck-tunic?color=6CQ
+https://staging-ecomm.jjill.com/product/long-sleeve-pima-crew-neck-tee?color=6ZV
+https://staging-ecomm.jjill.com/product/fit-french-terry-seamed-sweatshirt?color=AZN
+https://staging-ecomm.jjill.com/product/fit-hooded-snap-front-tunic?color=6EI
+https://staging-ecomm.jjill.com/product/fit-ultimate-fleece-collared-sweatshirt?color=871
+https://staging-ecomm.jjill.com/product/essential-forward-seam-tee?color=6TD
+https://staging-ecomm.jjill.com/product/twisted-hem-heathered-top?color=6SS
+https://staging-ecomm.jjill.com/product/striped-a-line-halter-top?color=6CC
+https://staging-ecomm.jjill.com/product/wearever-shirred-a-line-tunic?color=6DB
+https://staging-ecomm.jjill.com/product/pima-slub-elbow-sleeve-tee?color=0SY
+https://staging-ecomm.jjill.com/product/wearever-convertible-shoulder-top?color=31J
+https://staging-ecomm.jjill.com/product/wearever-double-face-jersey-seamed-tee?color=20M
+https://staging-ecomm.jjill.com/product/pure-jill-hemp-cotton-henley-top?color=61F
+https://staging-ecomm.jjill.com/product/pure-jill-space-dyed-tunic?color=347
+https://staging-ecomm.jjill.com/product/pure-jill-double-knit-seamed-tunic?color=6AW
+https://staging-ecomm.jjill.com/product/pure-jill-printed-soft-v-neck-top?color=6CZ
+https://staging-ecomm.jjill.com/product/pure-jill-banded-embroidered-tee?color=6SN
+https://staging-ecomm.jjill.com/product/wearever-convertible-shoulder-smocked-neck-top?color=6GS
+https://staging-ecomm.jjill.com/product/fit-progress-pima-stretch-shirttail-te-132651s-1?color=67Q
+</t>
+  </si>
 </sst>
 </file>
 
@@ -293,7 +663,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -349,12 +719,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -403,6 +786,9 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="1" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -419,10 +805,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -728,20 +1110,20 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.453125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="12" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.08984375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" style="2" customWidth="1"/>
-    <col min="6" max="7" width="8.7265625" style="2"/>
+    <col min="3" max="3" width="12.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" style="2" customWidth="1"/>
+    <col min="6" max="7" width="8.77734375" style="2"/>
     <col min="8" max="8" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="2"/>
+    <col min="9" max="9" width="22.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -770,7 +1152,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>49</v>
       </c>
@@ -813,19 +1195,19 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="12.6328125" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -845,7 +1227,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>33</v>
       </c>
@@ -865,7 +1247,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
@@ -885,7 +1267,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>56</v>
       </c>
@@ -921,20 +1303,20 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7265625" customWidth="1"/>
-    <col min="3" max="3" width="19.08984375" style="9" customWidth="1"/>
-    <col min="4" max="4" width="17.90625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="24.36328125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="22.54296875" style="9" customWidth="1"/>
-    <col min="7" max="7" width="24.81640625" style="9" customWidth="1"/>
-    <col min="8" max="8" width="22.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="22.5546875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="24.77734375" style="9" customWidth="1"/>
+    <col min="8" max="8" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -963,7 +1345,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" s="11" customFormat="1" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>52</v>
       </c>
@@ -992,7 +1374,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H3" s="18"/>
     </row>
   </sheetData>
@@ -1005,19 +1387,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA23885-4FA5-45F3-86BB-5039FDA0F69E}">
   <dimension ref="A1:XFD12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.21875" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" style="13"/>
+    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1037,7 +1419,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>31</v>
       </c>
@@ -1051,7 +1433,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="15"/>
     </row>
-    <row r="3" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>34</v>
       </c>
@@ -17443,7 +17825,7 @@
       <c r="XFC3" s="6"/>
       <c r="XFD3" s="3"/>
     </row>
-    <row r="4" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>35</v>
       </c>
@@ -17463,7 +17845,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>36</v>
       </c>
@@ -17483,7 +17865,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>37</v>
       </c>
@@ -17503,7 +17885,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>65</v>
       </c>
@@ -17517,12 +17899,12 @@
       <c r="E7" s="8"/>
       <c r="F7" s="15"/>
     </row>
-    <row r="11" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="C11" s="22" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="C12" s="23" t="s">
         <v>67</v>
       </c>
@@ -17531,4 +17913,122 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FF20DC2-8F2E-4969-821C-F8EB148B52AB}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="83.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>